<commit_message>
Mise à jour de Gantt
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="13370" tabRatio="415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8980" windowHeight="4190" tabRatio="415"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -179,10 +179,61 @@
     <t>Développement du site internet</t>
   </si>
   <si>
-    <t>LIGNANI</t>
+    <t>Modélisation du diagramme UML</t>
   </si>
   <si>
-    <t>Modélisation du diagramme UML</t>
+    <t xml:space="preserve">Site internet accessible sur téléphone </t>
+  </si>
+  <si>
+    <t>Portage du site internet afin de le rendre utilisable sur un téléphone portable</t>
+  </si>
+  <si>
+    <t>Test d’utilisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rédaction de la documentation </t>
+  </si>
+  <si>
+    <t>Création du panel administrateur</t>
+  </si>
+  <si>
+    <t>Prototypage de la vue administrateur</t>
+  </si>
+  <si>
+    <t>Accès aux données voulues</t>
+  </si>
+  <si>
+    <t>Envoie de message aux membres inscrits</t>
+  </si>
+  <si>
+    <t>Envoie de mail aux membres inscrits</t>
+  </si>
+  <si>
+    <t>Visibilité des données souhaitées</t>
+  </si>
+  <si>
+    <t>Exportation des données sous format Excel</t>
+  </si>
+  <si>
+    <t>Installation d’un serveur Web</t>
+  </si>
+  <si>
+    <t>Permettre aux utilisateurs d’ajouter mes messages en favoris</t>
+  </si>
+  <si>
+    <t>Ajouter la possibilité de créer des groupes privés</t>
+  </si>
+  <si>
+    <t>Ajouter une barre de notification (message privé, message de la direction…)</t>
+  </si>
+  <si>
+    <t>LOIC</t>
+  </si>
+  <si>
+    <t>QUENTIN</t>
+  </si>
+  <si>
+    <t>AMINE</t>
   </si>
 </sst>
 </file>
@@ -195,7 +246,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="d"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="8" tint="-0.499984740745262"/>
@@ -421,6 +472,47 @@
       <b/>
       <sz val="12"/>
       <color theme="8" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1002,7 +1094,7 @@
     <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1167,6 +1259,21 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="20 % - Accent1" xfId="27" builtinId="30" customBuiltin="1"/>
@@ -1222,6 +1329,19 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="8" tint="-0.499984740745262"/>
@@ -1255,19 +1375,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <right/>
       </border>
     </dxf>
     <dxf>
@@ -1570,8 +1677,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Jalons" displayName="Jalons" ref="B6:F24" totalsRowShown="0">
-  <autoFilter ref="B6:F24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Jalons" displayName="Jalons" ref="B6:F40" totalsRowShown="0">
+  <autoFilter ref="B6:F40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1860,10 +1967,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BK27"/>
+  <dimension ref="A1:BK43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2817,10 +2924,10 @@
         <v>22</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D9" s="24">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="25">
         <f ca="1">TODAY()</f>
@@ -3060,7 +3167,9 @@
       <c r="B10" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="27" t="s">
+        <v>57</v>
+      </c>
       <c r="D10" s="24">
         <v>1</v>
       </c>
@@ -3301,7 +3410,9 @@
       <c r="B11" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="27" t="s">
+        <v>59</v>
+      </c>
       <c r="D11" s="24">
         <v>1</v>
       </c>
@@ -3540,20 +3651,24 @@
     <row r="12" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12"/>
       <c r="B12" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>58</v>
+      </c>
       <c r="D12" s="24">
-        <v>0</v>
-      </c>
-      <c r="E12" s="25"/>
+        <v>0.2</v>
+      </c>
+      <c r="E12" s="25">
+        <v>44081</v>
+      </c>
       <c r="F12" s="48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="20"/>
-      <c r="H12" s="29" t="str">
+      <c r="H12" s="29">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="I12" s="29" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
@@ -3781,7 +3896,9 @@
       <c r="B13" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="27" t="s">
+        <v>57</v>
+      </c>
       <c r="D13" s="24">
         <v>0.5</v>
       </c>
@@ -5573,311 +5690,1410 @@
         <v>0</v>
       </c>
       <c r="E24" s="25"/>
-      <c r="F24" s="48">
+      <c r="F24" s="48"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="29"/>
+      <c r="X24" s="29"/>
+      <c r="Y24" s="29"/>
+      <c r="Z24" s="29"/>
+      <c r="AA24" s="29"/>
+      <c r="AB24" s="29"/>
+      <c r="AC24" s="29"/>
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="29"/>
+      <c r="AF24" s="29"/>
+      <c r="AG24" s="29"/>
+      <c r="AH24" s="29"/>
+      <c r="AI24" s="29"/>
+      <c r="AJ24" s="29"/>
+      <c r="AK24" s="29"/>
+      <c r="AL24" s="29"/>
+      <c r="AM24" s="29"/>
+      <c r="AN24" s="29"/>
+      <c r="AO24" s="29"/>
+      <c r="AP24" s="29"/>
+      <c r="AQ24" s="29"/>
+      <c r="AR24" s="29"/>
+      <c r="AS24" s="29"/>
+      <c r="AT24" s="29"/>
+      <c r="AU24" s="29"/>
+      <c r="AV24" s="29"/>
+      <c r="AW24" s="29"/>
+      <c r="AX24" s="29"/>
+      <c r="AY24" s="29"/>
+      <c r="AZ24" s="29"/>
+      <c r="BA24" s="29"/>
+      <c r="BB24" s="29"/>
+      <c r="BC24" s="29"/>
+      <c r="BD24" s="29"/>
+      <c r="BE24" s="29"/>
+      <c r="BF24" s="29"/>
+      <c r="BG24" s="29"/>
+      <c r="BH24" s="29"/>
+      <c r="BI24" s="29"/>
+      <c r="BJ24" s="29"/>
+      <c r="BK24" s="29"/>
+    </row>
+    <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="12"/>
+      <c r="B25" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="65"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
+      <c r="T25" s="29"/>
+      <c r="U25" s="29"/>
+      <c r="V25" s="29"/>
+      <c r="W25" s="29"/>
+      <c r="X25" s="29"/>
+      <c r="Y25" s="29"/>
+      <c r="Z25" s="29"/>
+      <c r="AA25" s="29"/>
+      <c r="AB25" s="29"/>
+      <c r="AC25" s="29"/>
+      <c r="AD25" s="29"/>
+      <c r="AE25" s="29"/>
+      <c r="AF25" s="29"/>
+      <c r="AG25" s="29"/>
+      <c r="AH25" s="29"/>
+      <c r="AI25" s="29"/>
+      <c r="AJ25" s="29"/>
+      <c r="AK25" s="29"/>
+      <c r="AL25" s="29"/>
+      <c r="AM25" s="29"/>
+      <c r="AN25" s="29"/>
+      <c r="AO25" s="29"/>
+      <c r="AP25" s="29"/>
+      <c r="AQ25" s="29"/>
+      <c r="AR25" s="29"/>
+      <c r="AS25" s="29"/>
+      <c r="AT25" s="29"/>
+      <c r="AU25" s="29"/>
+      <c r="AV25" s="29"/>
+      <c r="AW25" s="29"/>
+      <c r="AX25" s="29"/>
+      <c r="AY25" s="29"/>
+      <c r="AZ25" s="29"/>
+      <c r="BA25" s="29"/>
+      <c r="BB25" s="29"/>
+      <c r="BC25" s="29"/>
+      <c r="BD25" s="29"/>
+      <c r="BE25" s="29"/>
+      <c r="BF25" s="29"/>
+      <c r="BG25" s="29"/>
+      <c r="BH25" s="29"/>
+      <c r="BI25" s="29"/>
+      <c r="BJ25" s="29"/>
+      <c r="BK25" s="29"/>
+    </row>
+    <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="12"/>
+      <c r="B26" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="24">
         <v>0</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="I24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="J24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="K24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="L24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="M24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="N24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="O24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="P24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Q24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="R24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="S24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="T24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="U24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="V24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="W24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="X24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Y24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Z24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AA24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AB24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AC24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AD24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AE24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AF24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AG24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AH24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AI24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AJ24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AK24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AL24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AM24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AN24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AO24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AP24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AQ24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AR24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AS24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AT24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AU24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AV24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AW24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AX24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AY24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AZ24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BA24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BB24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BC24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BD24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BE24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BF24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BG24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BH24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BI24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BJ24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BK24" s="29" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E24,$F24=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
+      <c r="V26" s="29"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
+      <c r="Y26" s="29"/>
+      <c r="Z26" s="29"/>
+      <c r="AA26" s="29"/>
+      <c r="AB26" s="29"/>
+      <c r="AC26" s="29"/>
+      <c r="AD26" s="29"/>
+      <c r="AE26" s="29"/>
+      <c r="AF26" s="29"/>
+      <c r="AG26" s="29"/>
+      <c r="AH26" s="29"/>
+      <c r="AI26" s="29"/>
+      <c r="AJ26" s="29"/>
+      <c r="AK26" s="29"/>
+      <c r="AL26" s="29"/>
+      <c r="AM26" s="29"/>
+      <c r="AN26" s="29"/>
+      <c r="AO26" s="29"/>
+      <c r="AP26" s="29"/>
+      <c r="AQ26" s="29"/>
+      <c r="AR26" s="29"/>
+      <c r="AS26" s="29"/>
+      <c r="AT26" s="29"/>
+      <c r="AU26" s="29"/>
+      <c r="AV26" s="29"/>
+      <c r="AW26" s="29"/>
+      <c r="AX26" s="29"/>
+      <c r="AY26" s="29"/>
+      <c r="AZ26" s="29"/>
+      <c r="BA26" s="29"/>
+      <c r="BB26" s="29"/>
+      <c r="BC26" s="29"/>
+      <c r="BD26" s="29"/>
+      <c r="BE26" s="29"/>
+      <c r="BF26" s="29"/>
+      <c r="BG26" s="29"/>
+      <c r="BH26" s="29"/>
+      <c r="BI26" s="29"/>
+      <c r="BJ26" s="29"/>
+      <c r="BK26" s="29"/>
     </row>
-    <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="13" t="s">
+    <row r="27" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="12"/>
+      <c r="B27" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="27"/>
+      <c r="D27" s="24">
+        <v>0</v>
+      </c>
+      <c r="E27" s="25"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29"/>
+      <c r="AA27" s="29"/>
+      <c r="AB27" s="29"/>
+      <c r="AC27" s="29"/>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="29"/>
+      <c r="AG27" s="29"/>
+      <c r="AH27" s="29"/>
+      <c r="AI27" s="29"/>
+      <c r="AJ27" s="29"/>
+      <c r="AK27" s="29"/>
+      <c r="AL27" s="29"/>
+      <c r="AM27" s="29"/>
+      <c r="AN27" s="29"/>
+      <c r="AO27" s="29"/>
+      <c r="AP27" s="29"/>
+      <c r="AQ27" s="29"/>
+      <c r="AR27" s="29"/>
+      <c r="AS27" s="29"/>
+      <c r="AT27" s="29"/>
+      <c r="AU27" s="29"/>
+      <c r="AV27" s="29"/>
+      <c r="AW27" s="29"/>
+      <c r="AX27" s="29"/>
+      <c r="AY27" s="29"/>
+      <c r="AZ27" s="29"/>
+      <c r="BA27" s="29"/>
+      <c r="BB27" s="29"/>
+      <c r="BC27" s="29"/>
+      <c r="BD27" s="29"/>
+      <c r="BE27" s="29"/>
+      <c r="BF27" s="29"/>
+      <c r="BG27" s="29"/>
+      <c r="BH27" s="29"/>
+      <c r="BI27" s="29"/>
+      <c r="BJ27" s="29"/>
+      <c r="BK27" s="29"/>
+    </row>
+    <row r="28" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="12"/>
+      <c r="B28" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="27"/>
+      <c r="D28" s="24">
+        <v>0</v>
+      </c>
+      <c r="E28" s="25"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
+      <c r="U28" s="29"/>
+      <c r="V28" s="29"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="29"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29"/>
+      <c r="AA28" s="29"/>
+      <c r="AB28" s="29"/>
+      <c r="AC28" s="29"/>
+      <c r="AD28" s="29"/>
+      <c r="AE28" s="29"/>
+      <c r="AF28" s="29"/>
+      <c r="AG28" s="29"/>
+      <c r="AH28" s="29"/>
+      <c r="AI28" s="29"/>
+      <c r="AJ28" s="29"/>
+      <c r="AK28" s="29"/>
+      <c r="AL28" s="29"/>
+      <c r="AM28" s="29"/>
+      <c r="AN28" s="29"/>
+      <c r="AO28" s="29"/>
+      <c r="AP28" s="29"/>
+      <c r="AQ28" s="29"/>
+      <c r="AR28" s="29"/>
+      <c r="AS28" s="29"/>
+      <c r="AT28" s="29"/>
+      <c r="AU28" s="29"/>
+      <c r="AV28" s="29"/>
+      <c r="AW28" s="29"/>
+      <c r="AX28" s="29"/>
+      <c r="AY28" s="29"/>
+      <c r="AZ28" s="29"/>
+      <c r="BA28" s="29"/>
+      <c r="BB28" s="29"/>
+      <c r="BC28" s="29"/>
+      <c r="BD28" s="29"/>
+      <c r="BE28" s="29"/>
+      <c r="BF28" s="29"/>
+      <c r="BG28" s="29"/>
+      <c r="BH28" s="29"/>
+      <c r="BI28" s="29"/>
+      <c r="BJ28" s="29"/>
+      <c r="BK28" s="29"/>
+    </row>
+    <row r="29" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="12"/>
+      <c r="B29" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="27"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="29"/>
+      <c r="U29" s="29"/>
+      <c r="V29" s="29"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="29"/>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="29"/>
+      <c r="AA29" s="29"/>
+      <c r="AB29" s="29"/>
+      <c r="AC29" s="29"/>
+      <c r="AD29" s="29"/>
+      <c r="AE29" s="29"/>
+      <c r="AF29" s="29"/>
+      <c r="AG29" s="29"/>
+      <c r="AH29" s="29"/>
+      <c r="AI29" s="29"/>
+      <c r="AJ29" s="29"/>
+      <c r="AK29" s="29"/>
+      <c r="AL29" s="29"/>
+      <c r="AM29" s="29"/>
+      <c r="AN29" s="29"/>
+      <c r="AO29" s="29"/>
+      <c r="AP29" s="29"/>
+      <c r="AQ29" s="29"/>
+      <c r="AR29" s="29"/>
+      <c r="AS29" s="29"/>
+      <c r="AT29" s="29"/>
+      <c r="AU29" s="29"/>
+      <c r="AV29" s="29"/>
+      <c r="AW29" s="29"/>
+      <c r="AX29" s="29"/>
+      <c r="AY29" s="29"/>
+      <c r="AZ29" s="29"/>
+      <c r="BA29" s="29"/>
+      <c r="BB29" s="29"/>
+      <c r="BC29" s="29"/>
+      <c r="BD29" s="29"/>
+      <c r="BE29" s="29"/>
+      <c r="BF29" s="29"/>
+      <c r="BG29" s="29"/>
+      <c r="BH29" s="29"/>
+      <c r="BI29" s="29"/>
+      <c r="BJ29" s="29"/>
+      <c r="BK29" s="29"/>
+    </row>
+    <row r="30" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="12"/>
+      <c r="B30" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="27"/>
+      <c r="D30" s="24">
+        <v>0</v>
+      </c>
+      <c r="E30" s="25"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+      <c r="T30" s="29"/>
+      <c r="U30" s="29"/>
+      <c r="V30" s="29"/>
+      <c r="W30" s="29"/>
+      <c r="X30" s="29"/>
+      <c r="Y30" s="29"/>
+      <c r="Z30" s="29"/>
+      <c r="AA30" s="29"/>
+      <c r="AB30" s="29"/>
+      <c r="AC30" s="29"/>
+      <c r="AD30" s="29"/>
+      <c r="AE30" s="29"/>
+      <c r="AF30" s="29"/>
+      <c r="AG30" s="29"/>
+      <c r="AH30" s="29"/>
+      <c r="AI30" s="29"/>
+      <c r="AJ30" s="29"/>
+      <c r="AK30" s="29"/>
+      <c r="AL30" s="29"/>
+      <c r="AM30" s="29"/>
+      <c r="AN30" s="29"/>
+      <c r="AO30" s="29"/>
+      <c r="AP30" s="29"/>
+      <c r="AQ30" s="29"/>
+      <c r="AR30" s="29"/>
+      <c r="AS30" s="29"/>
+      <c r="AT30" s="29"/>
+      <c r="AU30" s="29"/>
+      <c r="AV30" s="29"/>
+      <c r="AW30" s="29"/>
+      <c r="AX30" s="29"/>
+      <c r="AY30" s="29"/>
+      <c r="AZ30" s="29"/>
+      <c r="BA30" s="29"/>
+      <c r="BB30" s="29"/>
+      <c r="BC30" s="29"/>
+      <c r="BD30" s="29"/>
+      <c r="BE30" s="29"/>
+      <c r="BF30" s="29"/>
+      <c r="BG30" s="29"/>
+      <c r="BH30" s="29"/>
+      <c r="BI30" s="29"/>
+      <c r="BJ30" s="29"/>
+      <c r="BK30" s="29"/>
+    </row>
+    <row r="31" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="12"/>
+      <c r="B31" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="27"/>
+      <c r="D31" s="24">
+        <v>0</v>
+      </c>
+      <c r="E31" s="25"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="29"/>
+      <c r="S31" s="29"/>
+      <c r="T31" s="29"/>
+      <c r="U31" s="29"/>
+      <c r="V31" s="29"/>
+      <c r="W31" s="29"/>
+      <c r="X31" s="29"/>
+      <c r="Y31" s="29"/>
+      <c r="Z31" s="29"/>
+      <c r="AA31" s="29"/>
+      <c r="AB31" s="29"/>
+      <c r="AC31" s="29"/>
+      <c r="AD31" s="29"/>
+      <c r="AE31" s="29"/>
+      <c r="AF31" s="29"/>
+      <c r="AG31" s="29"/>
+      <c r="AH31" s="29"/>
+      <c r="AI31" s="29"/>
+      <c r="AJ31" s="29"/>
+      <c r="AK31" s="29"/>
+      <c r="AL31" s="29"/>
+      <c r="AM31" s="29"/>
+      <c r="AN31" s="29"/>
+      <c r="AO31" s="29"/>
+      <c r="AP31" s="29"/>
+      <c r="AQ31" s="29"/>
+      <c r="AR31" s="29"/>
+      <c r="AS31" s="29"/>
+      <c r="AT31" s="29"/>
+      <c r="AU31" s="29"/>
+      <c r="AV31" s="29"/>
+      <c r="AW31" s="29"/>
+      <c r="AX31" s="29"/>
+      <c r="AY31" s="29"/>
+      <c r="AZ31" s="29"/>
+      <c r="BA31" s="29"/>
+      <c r="BB31" s="29"/>
+      <c r="BC31" s="29"/>
+      <c r="BD31" s="29"/>
+      <c r="BE31" s="29"/>
+      <c r="BF31" s="29"/>
+      <c r="BG31" s="29"/>
+      <c r="BH31" s="29"/>
+      <c r="BI31" s="29"/>
+      <c r="BJ31" s="29"/>
+      <c r="BK31" s="29"/>
+    </row>
+    <row r="32" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="12"/>
+      <c r="B32" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="D32" s="24">
+        <v>0</v>
+      </c>
+      <c r="E32" s="25"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
+      <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
+      <c r="S32" s="29"/>
+      <c r="T32" s="29"/>
+      <c r="U32" s="29"/>
+      <c r="V32" s="29"/>
+      <c r="W32" s="29"/>
+      <c r="X32" s="29"/>
+      <c r="Y32" s="29"/>
+      <c r="Z32" s="29"/>
+      <c r="AA32" s="29"/>
+      <c r="AB32" s="29"/>
+      <c r="AC32" s="29"/>
+      <c r="AD32" s="29"/>
+      <c r="AE32" s="29"/>
+      <c r="AF32" s="29"/>
+      <c r="AG32" s="29"/>
+      <c r="AH32" s="29"/>
+      <c r="AI32" s="29"/>
+      <c r="AJ32" s="29"/>
+      <c r="AK32" s="29"/>
+      <c r="AL32" s="29"/>
+      <c r="AM32" s="29"/>
+      <c r="AN32" s="29"/>
+      <c r="AO32" s="29"/>
+      <c r="AP32" s="29"/>
+      <c r="AQ32" s="29"/>
+      <c r="AR32" s="29"/>
+      <c r="AS32" s="29"/>
+      <c r="AT32" s="29"/>
+      <c r="AU32" s="29"/>
+      <c r="AV32" s="29"/>
+      <c r="AW32" s="29"/>
+      <c r="AX32" s="29"/>
+      <c r="AY32" s="29"/>
+      <c r="AZ32" s="29"/>
+      <c r="BA32" s="29"/>
+      <c r="BB32" s="29"/>
+      <c r="BC32" s="29"/>
+      <c r="BD32" s="29"/>
+      <c r="BE32" s="29"/>
+      <c r="BF32" s="29"/>
+      <c r="BG32" s="29"/>
+      <c r="BH32" s="29"/>
+      <c r="BI32" s="29"/>
+      <c r="BJ32" s="29"/>
+      <c r="BK32" s="29"/>
+    </row>
+    <row r="33" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="12"/>
+      <c r="B33" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="27"/>
+      <c r="D33" s="24">
+        <v>0</v>
+      </c>
+      <c r="E33" s="25"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="29"/>
+      <c r="S33" s="29"/>
+      <c r="T33" s="29"/>
+      <c r="U33" s="29"/>
+      <c r="V33" s="29"/>
+      <c r="W33" s="29"/>
+      <c r="X33" s="29"/>
+      <c r="Y33" s="29"/>
+      <c r="Z33" s="29"/>
+      <c r="AA33" s="29"/>
+      <c r="AB33" s="29"/>
+      <c r="AC33" s="29"/>
+      <c r="AD33" s="29"/>
+      <c r="AE33" s="29"/>
+      <c r="AF33" s="29"/>
+      <c r="AG33" s="29"/>
+      <c r="AH33" s="29"/>
+      <c r="AI33" s="29"/>
+      <c r="AJ33" s="29"/>
+      <c r="AK33" s="29"/>
+      <c r="AL33" s="29"/>
+      <c r="AM33" s="29"/>
+      <c r="AN33" s="29"/>
+      <c r="AO33" s="29"/>
+      <c r="AP33" s="29"/>
+      <c r="AQ33" s="29"/>
+      <c r="AR33" s="29"/>
+      <c r="AS33" s="29"/>
+      <c r="AT33" s="29"/>
+      <c r="AU33" s="29"/>
+      <c r="AV33" s="29"/>
+      <c r="AW33" s="29"/>
+      <c r="AX33" s="29"/>
+      <c r="AY33" s="29"/>
+      <c r="AZ33" s="29"/>
+      <c r="BA33" s="29"/>
+      <c r="BB33" s="29"/>
+      <c r="BC33" s="29"/>
+      <c r="BD33" s="29"/>
+      <c r="BE33" s="29"/>
+      <c r="BF33" s="29"/>
+      <c r="BG33" s="29"/>
+      <c r="BH33" s="29"/>
+      <c r="BI33" s="29"/>
+      <c r="BJ33" s="29"/>
+      <c r="BK33" s="29"/>
+    </row>
+    <row r="34" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="12"/>
+      <c r="B34" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="24">
+        <v>0</v>
+      </c>
+      <c r="E34" s="25"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="29"/>
+      <c r="R34" s="29"/>
+      <c r="S34" s="29"/>
+      <c r="T34" s="29"/>
+      <c r="U34" s="29"/>
+      <c r="V34" s="29"/>
+      <c r="W34" s="29"/>
+      <c r="X34" s="29"/>
+      <c r="Y34" s="29"/>
+      <c r="Z34" s="29"/>
+      <c r="AA34" s="29"/>
+      <c r="AB34" s="29"/>
+      <c r="AC34" s="29"/>
+      <c r="AD34" s="29"/>
+      <c r="AE34" s="29"/>
+      <c r="AF34" s="29"/>
+      <c r="AG34" s="29"/>
+      <c r="AH34" s="29"/>
+      <c r="AI34" s="29"/>
+      <c r="AJ34" s="29"/>
+      <c r="AK34" s="29"/>
+      <c r="AL34" s="29"/>
+      <c r="AM34" s="29"/>
+      <c r="AN34" s="29"/>
+      <c r="AO34" s="29"/>
+      <c r="AP34" s="29"/>
+      <c r="AQ34" s="29"/>
+      <c r="AR34" s="29"/>
+      <c r="AS34" s="29"/>
+      <c r="AT34" s="29"/>
+      <c r="AU34" s="29"/>
+      <c r="AV34" s="29"/>
+      <c r="AW34" s="29"/>
+      <c r="AX34" s="29"/>
+      <c r="AY34" s="29"/>
+      <c r="AZ34" s="29"/>
+      <c r="BA34" s="29"/>
+      <c r="BB34" s="29"/>
+      <c r="BC34" s="29"/>
+      <c r="BD34" s="29"/>
+      <c r="BE34" s="29"/>
+      <c r="BF34" s="29"/>
+      <c r="BG34" s="29"/>
+      <c r="BH34" s="29"/>
+      <c r="BI34" s="29"/>
+      <c r="BJ34" s="29"/>
+      <c r="BK34" s="29"/>
+    </row>
+    <row r="35" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="12"/>
+      <c r="B35" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="27"/>
+      <c r="D35" s="24">
+        <v>0</v>
+      </c>
+      <c r="E35" s="25"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
+      <c r="Q35" s="29"/>
+      <c r="R35" s="29"/>
+      <c r="S35" s="29"/>
+      <c r="T35" s="29"/>
+      <c r="U35" s="29"/>
+      <c r="V35" s="29"/>
+      <c r="W35" s="29"/>
+      <c r="X35" s="29"/>
+      <c r="Y35" s="29"/>
+      <c r="Z35" s="29"/>
+      <c r="AA35" s="29"/>
+      <c r="AB35" s="29"/>
+      <c r="AC35" s="29"/>
+      <c r="AD35" s="29"/>
+      <c r="AE35" s="29"/>
+      <c r="AF35" s="29"/>
+      <c r="AG35" s="29"/>
+      <c r="AH35" s="29"/>
+      <c r="AI35" s="29"/>
+      <c r="AJ35" s="29"/>
+      <c r="AK35" s="29"/>
+      <c r="AL35" s="29"/>
+      <c r="AM35" s="29"/>
+      <c r="AN35" s="29"/>
+      <c r="AO35" s="29"/>
+      <c r="AP35" s="29"/>
+      <c r="AQ35" s="29"/>
+      <c r="AR35" s="29"/>
+      <c r="AS35" s="29"/>
+      <c r="AT35" s="29"/>
+      <c r="AU35" s="29"/>
+      <c r="AV35" s="29"/>
+      <c r="AW35" s="29"/>
+      <c r="AX35" s="29"/>
+      <c r="AY35" s="29"/>
+      <c r="AZ35" s="29"/>
+      <c r="BA35" s="29"/>
+      <c r="BB35" s="29"/>
+      <c r="BC35" s="29"/>
+      <c r="BD35" s="29"/>
+      <c r="BE35" s="29"/>
+      <c r="BF35" s="29"/>
+      <c r="BG35" s="29"/>
+      <c r="BH35" s="29"/>
+      <c r="BI35" s="29"/>
+      <c r="BJ35" s="29"/>
+      <c r="BK35" s="29"/>
+    </row>
+    <row r="36" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="12"/>
+      <c r="B36" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="54"/>
+      <c r="D36" s="24">
+        <v>0</v>
+      </c>
+      <c r="E36" s="25"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="29"/>
+      <c r="R36" s="29"/>
+      <c r="S36" s="29"/>
+      <c r="T36" s="29"/>
+      <c r="U36" s="29"/>
+      <c r="V36" s="29"/>
+      <c r="W36" s="29"/>
+      <c r="X36" s="29"/>
+      <c r="Y36" s="29"/>
+      <c r="Z36" s="29"/>
+      <c r="AA36" s="29"/>
+      <c r="AB36" s="29"/>
+      <c r="AC36" s="29"/>
+      <c r="AD36" s="29"/>
+      <c r="AE36" s="29"/>
+      <c r="AF36" s="29"/>
+      <c r="AG36" s="29"/>
+      <c r="AH36" s="29"/>
+      <c r="AI36" s="29"/>
+      <c r="AJ36" s="29"/>
+      <c r="AK36" s="29"/>
+      <c r="AL36" s="29"/>
+      <c r="AM36" s="29"/>
+      <c r="AN36" s="29"/>
+      <c r="AO36" s="29"/>
+      <c r="AP36" s="29"/>
+      <c r="AQ36" s="29"/>
+      <c r="AR36" s="29"/>
+      <c r="AS36" s="29"/>
+      <c r="AT36" s="29"/>
+      <c r="AU36" s="29"/>
+      <c r="AV36" s="29"/>
+      <c r="AW36" s="29"/>
+      <c r="AX36" s="29"/>
+      <c r="AY36" s="29"/>
+      <c r="AZ36" s="29"/>
+      <c r="BA36" s="29"/>
+      <c r="BB36" s="29"/>
+      <c r="BC36" s="29"/>
+      <c r="BD36" s="29"/>
+      <c r="BE36" s="29"/>
+      <c r="BF36" s="29"/>
+      <c r="BG36" s="29"/>
+      <c r="BH36" s="29"/>
+      <c r="BI36" s="29"/>
+      <c r="BJ36" s="29"/>
+      <c r="BK36" s="29"/>
+    </row>
+    <row r="37" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="12"/>
+      <c r="B37" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="54"/>
+      <c r="D37" s="24">
+        <v>0</v>
+      </c>
+      <c r="E37" s="25"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29"/>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="29"/>
+      <c r="AF37" s="29"/>
+      <c r="AG37" s="29"/>
+      <c r="AH37" s="29"/>
+      <c r="AI37" s="29"/>
+      <c r="AJ37" s="29"/>
+      <c r="AK37" s="29"/>
+      <c r="AL37" s="29"/>
+      <c r="AM37" s="29"/>
+      <c r="AN37" s="29"/>
+      <c r="AO37" s="29"/>
+      <c r="AP37" s="29"/>
+      <c r="AQ37" s="29"/>
+      <c r="AR37" s="29"/>
+      <c r="AS37" s="29"/>
+      <c r="AT37" s="29"/>
+      <c r="AU37" s="29"/>
+      <c r="AV37" s="29"/>
+      <c r="AW37" s="29"/>
+      <c r="AX37" s="29"/>
+      <c r="AY37" s="29"/>
+      <c r="AZ37" s="29"/>
+      <c r="BA37" s="29"/>
+      <c r="BB37" s="29"/>
+      <c r="BC37" s="29"/>
+      <c r="BD37" s="29"/>
+      <c r="BE37" s="29"/>
+      <c r="BF37" s="29"/>
+      <c r="BG37" s="29"/>
+      <c r="BH37" s="29"/>
+      <c r="BI37" s="29"/>
+      <c r="BJ37" s="29"/>
+      <c r="BK37" s="29"/>
+    </row>
+    <row r="38" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="12"/>
+      <c r="B38" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="54"/>
+      <c r="D38" s="24">
+        <v>0</v>
+      </c>
+      <c r="E38" s="25"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="29"/>
+      <c r="AF38" s="29"/>
+      <c r="AG38" s="29"/>
+      <c r="AH38" s="29"/>
+      <c r="AI38" s="29"/>
+      <c r="AJ38" s="29"/>
+      <c r="AK38" s="29"/>
+      <c r="AL38" s="29"/>
+      <c r="AM38" s="29"/>
+      <c r="AN38" s="29"/>
+      <c r="AO38" s="29"/>
+      <c r="AP38" s="29"/>
+      <c r="AQ38" s="29"/>
+      <c r="AR38" s="29"/>
+      <c r="AS38" s="29"/>
+      <c r="AT38" s="29"/>
+      <c r="AU38" s="29"/>
+      <c r="AV38" s="29"/>
+      <c r="AW38" s="29"/>
+      <c r="AX38" s="29"/>
+      <c r="AY38" s="29"/>
+      <c r="AZ38" s="29"/>
+      <c r="BA38" s="29"/>
+      <c r="BB38" s="29"/>
+      <c r="BC38" s="29"/>
+      <c r="BD38" s="29"/>
+      <c r="BE38" s="29"/>
+      <c r="BF38" s="29"/>
+      <c r="BG38" s="29"/>
+      <c r="BH38" s="29"/>
+      <c r="BI38" s="29"/>
+      <c r="BJ38" s="29"/>
+      <c r="BK38" s="29"/>
+    </row>
+    <row r="39" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="12"/>
+      <c r="B39" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="68"/>
+      <c r="D39" s="24">
+        <v>0</v>
+      </c>
+      <c r="E39" s="25"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="29"/>
+      <c r="Q39" s="29"/>
+      <c r="R39" s="29"/>
+      <c r="S39" s="29"/>
+      <c r="T39" s="29"/>
+      <c r="U39" s="29"/>
+      <c r="V39" s="29"/>
+      <c r="W39" s="29"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="29"/>
+      <c r="AC39" s="29"/>
+      <c r="AD39" s="29"/>
+      <c r="AE39" s="29"/>
+      <c r="AF39" s="29"/>
+      <c r="AG39" s="29"/>
+      <c r="AH39" s="29"/>
+      <c r="AI39" s="29"/>
+      <c r="AJ39" s="29"/>
+      <c r="AK39" s="29"/>
+      <c r="AL39" s="29"/>
+      <c r="AM39" s="29"/>
+      <c r="AN39" s="29"/>
+      <c r="AO39" s="29"/>
+      <c r="AP39" s="29"/>
+      <c r="AQ39" s="29"/>
+      <c r="AR39" s="29"/>
+      <c r="AS39" s="29"/>
+      <c r="AT39" s="29"/>
+      <c r="AU39" s="29"/>
+      <c r="AV39" s="29"/>
+      <c r="AW39" s="29"/>
+      <c r="AX39" s="29"/>
+      <c r="AY39" s="29"/>
+      <c r="AZ39" s="29"/>
+      <c r="BA39" s="29"/>
+      <c r="BB39" s="29"/>
+      <c r="BC39" s="29"/>
+      <c r="BD39" s="29"/>
+      <c r="BE39" s="29"/>
+      <c r="BF39" s="29"/>
+      <c r="BG39" s="29"/>
+      <c r="BH39" s="29"/>
+      <c r="BI39" s="29"/>
+      <c r="BJ39" s="29"/>
+      <c r="BK39" s="29"/>
+    </row>
+    <row r="40" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="12"/>
+      <c r="B40" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="24">
+        <v>0</v>
+      </c>
+      <c r="E40" s="25"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="I40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="J40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="K40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="L40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="M40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="N40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="O40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="P40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Q40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="R40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="S40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="T40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="U40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="V40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="W40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="X40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Y40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Z40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AA40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AB40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AC40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AD40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AE40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AF40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AG40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AH40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AI40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AJ40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AK40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AL40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AM40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AN40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AO40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AP40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AQ40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AR40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AS40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AT40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AU40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AV40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AW40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AX40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AY40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AZ40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BA40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BB40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BC40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BD40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BE40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BF40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BG40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BH40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BI40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BJ40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BK40" s="29" t="str">
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E40,$F40=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="12"/>
+      <c r="B41" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="28"/>
+      <c r="P41" s="28"/>
+      <c r="Q41" s="28"/>
+      <c r="R41" s="28"/>
+      <c r="S41" s="28"/>
+      <c r="T41" s="28"/>
+      <c r="U41" s="28"/>
+      <c r="V41" s="28"/>
+      <c r="W41" s="28"/>
+      <c r="X41" s="28"/>
+      <c r="Y41" s="28"/>
+      <c r="Z41" s="28"/>
+      <c r="AA41" s="28"/>
+      <c r="AB41" s="28"/>
+      <c r="AC41" s="28"/>
+      <c r="AD41" s="28"/>
+      <c r="AE41" s="28"/>
+      <c r="AF41" s="28"/>
+      <c r="AG41" s="28"/>
+      <c r="AH41" s="28"/>
+      <c r="AI41" s="28"/>
+      <c r="AJ41" s="28"/>
+      <c r="AK41" s="28"/>
+      <c r="AL41" s="28"/>
+      <c r="AM41" s="28"/>
+      <c r="AN41" s="28"/>
+      <c r="AO41" s="28"/>
+      <c r="AP41" s="28"/>
+      <c r="AQ41" s="28"/>
+      <c r="AR41" s="28"/>
+      <c r="AS41" s="28"/>
+      <c r="AT41" s="28"/>
+      <c r="AU41" s="28"/>
+      <c r="AV41" s="28"/>
+      <c r="AW41" s="28"/>
+      <c r="AX41" s="28"/>
+      <c r="AY41" s="28"/>
+      <c r="AZ41" s="28"/>
+      <c r="BA41" s="28"/>
+      <c r="BB41" s="28"/>
+      <c r="BC41" s="28"/>
+      <c r="BD41" s="28"/>
+      <c r="BE41" s="28"/>
+      <c r="BF41" s="28"/>
+      <c r="BG41" s="28"/>
+      <c r="BH41" s="28"/>
+      <c r="BI41" s="28"/>
+      <c r="BJ41" s="28"/>
+      <c r="BK41" s="28"/>
+    </row>
+    <row r="42" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C42" s="5"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="28"/>
-      <c r="U25" s="28"/>
-      <c r="V25" s="28"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="28"/>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="28"/>
-      <c r="AA25" s="28"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="28"/>
-      <c r="AD25" s="28"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
-      <c r="AG25" s="28"/>
-      <c r="AH25" s="28"/>
-      <c r="AI25" s="28"/>
-      <c r="AJ25" s="28"/>
-      <c r="AK25" s="28"/>
-      <c r="AL25" s="28"/>
-      <c r="AM25" s="28"/>
-      <c r="AN25" s="28"/>
-      <c r="AO25" s="28"/>
-      <c r="AP25" s="28"/>
-      <c r="AQ25" s="28"/>
-      <c r="AR25" s="28"/>
-      <c r="AS25" s="28"/>
-      <c r="AT25" s="28"/>
-      <c r="AU25" s="28"/>
-      <c r="AV25" s="28"/>
-      <c r="AW25" s="28"/>
-      <c r="AX25" s="28"/>
-      <c r="AY25" s="28"/>
-      <c r="AZ25" s="28"/>
-      <c r="BA25" s="28"/>
-      <c r="BB25" s="28"/>
-      <c r="BC25" s="28"/>
-      <c r="BD25" s="28"/>
-      <c r="BE25" s="28"/>
-      <c r="BF25" s="28"/>
-      <c r="BG25" s="28"/>
-      <c r="BH25" s="28"/>
-      <c r="BI25" s="28"/>
-      <c r="BJ25" s="28"/>
-      <c r="BK25" s="28"/>
-    </row>
-    <row r="26" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="5"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="6"/>
+      <c r="C43" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5886,7 +7102,7 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="C4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6:D24">
+  <conditionalFormatting sqref="D6:D40">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5900,18 +7116,18 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:BK24">
-    <cfRule type="expression" dxfId="1" priority="78">
+  <conditionalFormatting sqref="H8:BK40">
+    <cfRule type="expression" dxfId="2" priority="78">
       <formula>H$5&lt;=Aujourd’hui</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BK24">
-    <cfRule type="expression" dxfId="0" priority="11" stopIfTrue="1">
+  <conditionalFormatting sqref="H7:BK40">
+    <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
       <formula>AND(H$5&gt;=$E7+1,H$5&lt;=$E7+$F7-2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:BK6">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>H$5&lt;=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5975,7 +7191,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D6:D24</xm:sqref>
+          <xm:sqref>D6:D40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="2" id="{6C427F2E-2EF5-46B4-BFA6-7C68148277AC}">
@@ -6013,7 +7229,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H7:BK24</xm:sqref>
+          <xm:sqref>H7:BK40</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
ajout des sujets clairs pour chez nous
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C447FC-90AE-47B6-BB9F-257B43E9D3A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="415"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <definedName name="Incrément_Défilement">Gantt!$E$3</definedName>
     <definedName name="Marqueur_Jalon">Gantt!$E$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -255,7 +254,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
@@ -1305,7 +1304,7 @@
     <cellStyle name="Avertissement" xfId="23" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="20" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="21" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="9" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Date" xfId="9"/>
     <cellStyle name="Entrée" xfId="18" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="16" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -1327,7 +1326,7 @@
     <cellStyle name="Titre 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="25" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="22" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="zHiddenText" xfId="3"/>
   </cellStyles>
   <dxfs count="33">
     <dxf>
@@ -1871,12 +1870,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Gantt Table Style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Gantt Table Style" pivot="0" count="3">
       <tableStyleElement type="wholeTable" dxfId="32"/>
       <tableStyleElement type="headerRow" dxfId="31"/>
       <tableStyleElement type="firstRowStripe" dxfId="30"/>
     </tableStyle>
-    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="ToDoList" pivot="0" count="9">
       <tableStyleElement type="wholeTable" dxfId="29"/>
       <tableStyleElement type="headerRow" dxfId="28"/>
       <tableStyleElement type="totalRow" dxfId="27"/>
@@ -1980,11 +1979,11 @@
           <xdr:col>7</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>31750</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>180975</xdr:colOff>
+          <xdr:colOff>184150</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>342900</xdr:rowOff>
         </xdr:to>
@@ -2027,8 +2026,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Jalons" displayName="Jalons" ref="B6:F44" totalsRowShown="0">
-  <autoFilter ref="B6:F44" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Jalons" displayName="Jalons" ref="B6:F44" totalsRowShown="0">
+  <autoFilter ref="B6:F44">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2036,11 +2035,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Description du jalon"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Affecté à"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Avancement"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Début"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nombre de jours"/>
+    <tableColumn id="1" name="Description du jalon"/>
+    <tableColumn id="3" name="Affecté à"/>
+    <tableColumn id="4" name="Avancement"/>
+    <tableColumn id="5" name="Début"/>
+    <tableColumn id="6" name="Nombre de jours"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -2313,30 +2312,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BK46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AJ14" sqref="AJ14"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="3" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="63" width="3.5703125" customWidth="1"/>
-    <col min="68" max="69" width="10.28515625"/>
+    <col min="7" max="7" width="2.7265625" customWidth="1"/>
+    <col min="8" max="63" width="3.54296875" customWidth="1"/>
+    <col min="68" max="69" width="10.26953125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:63" ht="50.15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2349,7 +2348,7 @@
       <c r="I1" s="18"/>
       <c r="AF1" s="18"/>
     </row>
-    <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -2372,7 +2371,7 @@
       <c r="M2" s="32"/>
       <c r="N2" s="32"/>
     </row>
-    <row r="3" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
@@ -2393,7 +2392,7 @@
       <c r="L3" s="43"/>
       <c r="M3" s="42"/>
     </row>
-    <row r="4" spans="1:63" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:63" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
@@ -2489,7 +2488,7 @@
       <c r="BJ4" s="17"/>
       <c r="BK4" s="17"/>
     </row>
-    <row r="5" spans="1:63" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
@@ -2720,7 +2719,7 @@
         <v>44136</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:63" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -2965,7 +2964,7 @@
         <v>d</v>
       </c>
     </row>
-    <row r="7" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
@@ -3031,7 +3030,7 @@
       <c r="BJ7" s="37"/>
       <c r="BK7" s="37"/>
     </row>
-    <row r="8" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -3268,7 +3267,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="62" t="s">
         <v>21</v>
@@ -3511,7 +3510,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="28" t="s">
         <v>22</v>
@@ -3754,7 +3753,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
       <c r="B11" s="62" t="s">
         <v>23</v>
@@ -3997,7 +3996,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12"/>
       <c r="B12" s="28" t="s">
         <v>38</v>
@@ -4240,7 +4239,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12"/>
       <c r="B13" s="62" t="s">
         <v>24</v>
@@ -4483,7 +4482,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
       <c r="B14" s="53" t="s">
         <v>37</v>
@@ -4718,7 +4717,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="62" t="s">
         <v>26</v>
@@ -4961,7 +4960,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12"/>
       <c r="B16" s="50" t="s">
         <v>27</v>
@@ -5204,7 +5203,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12"/>
       <c r="B17" s="50" t="s">
         <v>28</v>
@@ -5447,7 +5446,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12"/>
       <c r="B18" s="50" t="s">
         <v>29</v>
@@ -5690,7 +5689,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12"/>
       <c r="B19" s="50" t="s">
         <v>30</v>
@@ -5765,7 +5764,7 @@
       <c r="BJ19" s="27"/>
       <c r="BK19" s="27"/>
     </row>
-    <row r="20" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12"/>
       <c r="B20" s="63" t="s">
         <v>32</v>
@@ -5840,7 +5839,7 @@
       <c r="BJ20" s="27"/>
       <c r="BK20" s="27"/>
     </row>
-    <row r="21" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12"/>
       <c r="B21" s="51" t="s">
         <v>33</v>
@@ -5918,7 +5917,7 @@
       <c r="BJ21" s="27"/>
       <c r="BK21" s="27"/>
     </row>
-    <row r="22" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12"/>
       <c r="B22" s="51" t="s">
         <v>57</v>
@@ -5993,7 +5992,7 @@
       <c r="BJ22" s="27"/>
       <c r="BK22" s="27"/>
     </row>
-    <row r="23" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12"/>
       <c r="B23" s="51" t="s">
         <v>62</v>
@@ -6066,7 +6065,7 @@
       <c r="BJ23" s="27"/>
       <c r="BK23" s="27"/>
     </row>
-    <row r="24" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="64" t="s">
         <v>63</v>
@@ -6141,7 +6140,7 @@
       <c r="BJ24" s="27"/>
       <c r="BK24" s="27"/>
     </row>
-    <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="64" t="s">
         <v>61</v>
@@ -6214,7 +6213,7 @@
       <c r="BJ25" s="27"/>
       <c r="BK25" s="27"/>
     </row>
-    <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
       <c r="B26" s="64" t="s">
         <v>64</v>
@@ -6287,7 +6286,7 @@
       <c r="BJ26" s="27"/>
       <c r="BK26" s="27"/>
     </row>
-    <row r="27" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12"/>
       <c r="B27" s="64" t="s">
         <v>31</v>
@@ -6360,7 +6359,7 @@
       <c r="BJ27" s="27"/>
       <c r="BK27" s="27"/>
     </row>
-    <row r="28" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12"/>
       <c r="B28" s="56" t="s">
         <v>39</v>
@@ -6427,7 +6426,7 @@
       <c r="BJ28" s="27"/>
       <c r="BK28" s="27"/>
     </row>
-    <row r="29" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12"/>
       <c r="B29" s="54" t="s">
         <v>40</v>
@@ -6502,7 +6501,7 @@
       <c r="BJ29" s="27"/>
       <c r="BK29" s="27"/>
     </row>
-    <row r="30" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12"/>
       <c r="B30" s="65" t="s">
         <v>41</v>
@@ -6571,7 +6570,7 @@
       <c r="BJ30" s="27"/>
       <c r="BK30" s="27"/>
     </row>
-    <row r="31" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12"/>
       <c r="B31" s="51" t="s">
         <v>42</v>
@@ -6640,7 +6639,7 @@
       <c r="BJ31" s="27"/>
       <c r="BK31" s="27"/>
     </row>
-    <row r="32" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12"/>
       <c r="B32" s="57" t="s">
         <v>43</v>
@@ -6707,7 +6706,7 @@
       <c r="BJ32" s="27"/>
       <c r="BK32" s="27"/>
     </row>
-    <row r="33" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12"/>
       <c r="B33" s="50" t="s">
         <v>44</v>
@@ -6776,7 +6775,7 @@
       <c r="BJ33" s="27"/>
       <c r="BK33" s="27"/>
     </row>
-    <row r="34" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12"/>
       <c r="B34" s="50" t="s">
         <v>45</v>
@@ -6845,7 +6844,7 @@
       <c r="BJ34" s="27"/>
       <c r="BK34" s="27"/>
     </row>
-    <row r="35" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="12"/>
       <c r="B35" s="51" t="s">
         <v>47</v>
@@ -6914,7 +6913,7 @@
       <c r="BJ35" s="27"/>
       <c r="BK35" s="27"/>
     </row>
-    <row r="36" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12"/>
       <c r="B36" s="64" t="s">
         <v>49</v>
@@ -6983,7 +6982,7 @@
       <c r="BJ36" s="27"/>
       <c r="BK36" s="27"/>
     </row>
-    <row r="37" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12"/>
       <c r="B37" s="51" t="s">
         <v>48</v>
@@ -7052,7 +7051,7 @@
       <c r="BJ37" s="27"/>
       <c r="BK37" s="27"/>
     </row>
-    <row r="38" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12"/>
       <c r="B38" s="51" t="s">
         <v>46</v>
@@ -7121,7 +7120,7 @@
       <c r="BJ38" s="27"/>
       <c r="BK38" s="27"/>
     </row>
-    <row r="39" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12"/>
       <c r="B39" s="50" t="s">
         <v>44</v>
@@ -7190,7 +7189,7 @@
       <c r="BJ39" s="27"/>
       <c r="BK39" s="27"/>
     </row>
-    <row r="40" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="12"/>
       <c r="B40" s="58" t="s">
         <v>50</v>
@@ -7427,7 +7426,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="12"/>
       <c r="B41" s="60" t="s">
         <v>51</v>
@@ -7664,7 +7663,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="59" t="s">
         <v>52</v>
       </c>
@@ -7676,7 +7675,7 @@
       <c r="F42" s="44"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
         <v>8</v>
       </c>
@@ -7690,7 +7689,7 @@
       <c r="E43" s="24"/>
       <c r="F43" s="44"/>
     </row>
-    <row r="44" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="66" t="s">
         <v>60</v>
       </c>
@@ -7707,11 +7706,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C45" s="5"/>
       <c r="F45" s="14"/>
     </row>
-    <row r="46" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C46" s="6"/>
     </row>
   </sheetData>
@@ -7855,7 +7854,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Incrément de défilement" prompt="La modification de ce nombre entraînera la défilement du diagramme de Gantt." sqref="E3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Incrément de défilement" prompt="La modification de ce nombre entraînera la défilement du diagramme de Gantt." sqref="E3">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -7879,11 +7878,11 @@
                     <xdr:col>7</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>31750</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>12</xdr:col>
-                    <xdr:colOff>180975</xdr:colOff>
+                    <xdr:colOff>184150</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>342900</xdr:rowOff>
                   </to>
@@ -7995,35 +7994,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.140625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="87.1796875" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="145" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" s="10" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Gantt à jour MATIN 27/10
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1988,7 +1988,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$E$3" horiz="1" max="365" page="0" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$E$3" horiz="1" max="365" page="0" val="25"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2339,8 +2339,8 @@
   </sheetPr>
   <dimension ref="A1:BK46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="L22" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="BF30" sqref="BF30"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2404,7 +2404,7 @@
       </c>
       <c r="D3" s="68"/>
       <c r="E3" s="35">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H3" s="42"/>
       <c r="I3" s="43"/>
@@ -2430,7 +2430,7 @@
       </c>
       <c r="H4" s="17" t="str">
         <f ca="1">TEXT(H5,"mmmm")</f>
-        <v>septembre</v>
+        <v>octobre</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
@@ -2470,7 +2470,7 @@
       <c r="AI4" s="17"/>
       <c r="AJ4" s="17" t="str">
         <f ca="1">IF(OR(TEXT(AJ5,"mmmm")=AC4,TEXT(AJ5,"mmmm")=V4,TEXT(AJ5,"mmmm")=O4,TEXT(AJ5,"mmmm")=H4),"",TEXT(AJ5,"mmmm"))</f>
-        <v>octobre</v>
+        <v/>
       </c>
       <c r="AK4" s="17"/>
       <c r="AL4" s="17"/>
@@ -2480,7 +2480,7 @@
       <c r="AP4" s="17"/>
       <c r="AQ4" s="17" t="str">
         <f ca="1">IF(OR(TEXT(AQ5,"mmmm")=AJ4,TEXT(AQ5,"mmmm")=AC4,TEXT(AQ5,"mmmm")=V4,TEXT(AQ5,"mmmm")=O4),"",TEXT(AQ5,"mmmm"))</f>
-        <v/>
+        <v>novembre</v>
       </c>
       <c r="AR4" s="17"/>
       <c r="AS4" s="17"/>
@@ -2517,227 +2517,227 @@
       <c r="G5" s="31"/>
       <c r="H5" s="45">
         <f ca="1">IFERROR(Début_Projet+Incrément_Défilement,TODAY())</f>
-        <v>44081</v>
+        <v>44106</v>
       </c>
       <c r="I5" s="46">
         <f ca="1">H5+1</f>
-        <v>44082</v>
+        <v>44107</v>
       </c>
       <c r="J5" s="47">
         <f t="shared" ref="J5:AW5" ca="1" si="0">I5+1</f>
-        <v>44083</v>
+        <v>44108</v>
       </c>
       <c r="K5" s="47">
         <f ca="1">J5+1</f>
-        <v>44084</v>
+        <v>44109</v>
       </c>
       <c r="L5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44085</v>
+        <v>44110</v>
       </c>
       <c r="M5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44086</v>
+        <v>44111</v>
       </c>
       <c r="N5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44087</v>
+        <v>44112</v>
       </c>
       <c r="O5" s="47">
         <f ca="1">N5+1</f>
-        <v>44088</v>
+        <v>44113</v>
       </c>
       <c r="P5" s="47">
         <f ca="1">O5+1</f>
-        <v>44089</v>
+        <v>44114</v>
       </c>
       <c r="Q5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44090</v>
+        <v>44115</v>
       </c>
       <c r="R5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44091</v>
+        <v>44116</v>
       </c>
       <c r="S5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44092</v>
+        <v>44117</v>
       </c>
       <c r="T5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44093</v>
+        <v>44118</v>
       </c>
       <c r="U5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44094</v>
+        <v>44119</v>
       </c>
       <c r="V5" s="47">
         <f ca="1">U5+1</f>
-        <v>44095</v>
+        <v>44120</v>
       </c>
       <c r="W5" s="47">
         <f ca="1">V5+1</f>
-        <v>44096</v>
+        <v>44121</v>
       </c>
       <c r="X5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44097</v>
+        <v>44122</v>
       </c>
       <c r="Y5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44098</v>
+        <v>44123</v>
       </c>
       <c r="Z5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44099</v>
+        <v>44124</v>
       </c>
       <c r="AA5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44100</v>
+        <v>44125</v>
       </c>
       <c r="AB5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44101</v>
+        <v>44126</v>
       </c>
       <c r="AC5" s="47">
         <f ca="1">AB5+1</f>
-        <v>44102</v>
+        <v>44127</v>
       </c>
       <c r="AD5" s="47">
         <f ca="1">AC5+1</f>
-        <v>44103</v>
+        <v>44128</v>
       </c>
       <c r="AE5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44104</v>
+        <v>44129</v>
       </c>
       <c r="AF5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44105</v>
+        <v>44130</v>
       </c>
       <c r="AG5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44106</v>
+        <v>44131</v>
       </c>
       <c r="AH5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44107</v>
+        <v>44132</v>
       </c>
       <c r="AI5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44108</v>
+        <v>44133</v>
       </c>
       <c r="AJ5" s="47">
         <f ca="1">AI5+1</f>
-        <v>44109</v>
+        <v>44134</v>
       </c>
       <c r="AK5" s="47">
         <f ca="1">AJ5+1</f>
-        <v>44110</v>
+        <v>44135</v>
       </c>
       <c r="AL5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44111</v>
+        <v>44136</v>
       </c>
       <c r="AM5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44112</v>
+        <v>44137</v>
       </c>
       <c r="AN5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44113</v>
+        <v>44138</v>
       </c>
       <c r="AO5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44114</v>
+        <v>44139</v>
       </c>
       <c r="AP5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44115</v>
+        <v>44140</v>
       </c>
       <c r="AQ5" s="47">
         <f ca="1">AP5+1</f>
-        <v>44116</v>
+        <v>44141</v>
       </c>
       <c r="AR5" s="47">
         <f ca="1">AQ5+1</f>
-        <v>44117</v>
+        <v>44142</v>
       </c>
       <c r="AS5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44118</v>
+        <v>44143</v>
       </c>
       <c r="AT5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44119</v>
+        <v>44144</v>
       </c>
       <c r="AU5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44120</v>
+        <v>44145</v>
       </c>
       <c r="AV5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44121</v>
+        <v>44146</v>
       </c>
       <c r="AW5" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44122</v>
+        <v>44147</v>
       </c>
       <c r="AX5" s="47">
         <f ca="1">AW5+1</f>
-        <v>44123</v>
+        <v>44148</v>
       </c>
       <c r="AY5" s="47">
         <f ca="1">AX5+1</f>
-        <v>44124</v>
+        <v>44149</v>
       </c>
       <c r="AZ5" s="47">
         <f t="shared" ref="AZ5:BD5" ca="1" si="1">AY5+1</f>
-        <v>44125</v>
+        <v>44150</v>
       </c>
       <c r="BA5" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>44126</v>
+        <v>44151</v>
       </c>
       <c r="BB5" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>44127</v>
+        <v>44152</v>
       </c>
       <c r="BC5" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>44128</v>
+        <v>44153</v>
       </c>
       <c r="BD5" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>44129</v>
+        <v>44154</v>
       </c>
       <c r="BE5" s="47">
         <f ca="1">BD5+1</f>
-        <v>44130</v>
+        <v>44155</v>
       </c>
       <c r="BF5" s="47">
         <f ca="1">BE5+1</f>
-        <v>44131</v>
+        <v>44156</v>
       </c>
       <c r="BG5" s="47">
         <f t="shared" ref="BG5:BK5" ca="1" si="2">BF5+1</f>
-        <v>44132</v>
+        <v>44157</v>
       </c>
       <c r="BH5" s="47">
         <f t="shared" ca="1" si="2"/>
-        <v>44133</v>
+        <v>44158</v>
       </c>
       <c r="BI5" s="47">
         <f t="shared" ca="1" si="2"/>
-        <v>44134</v>
+        <v>44159</v>
       </c>
       <c r="BJ5" s="47">
         <f t="shared" ca="1" si="2"/>
-        <v>44135</v>
+        <v>44160</v>
       </c>
       <c r="BK5" s="48">
         <f t="shared" ca="1" si="2"/>
-        <v>44136</v>
+        <v>44161</v>
       </c>
     </row>
     <row r="6" spans="1:63" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2762,227 +2762,227 @@
       <c r="G6" s="20"/>
       <c r="H6" s="38" t="str">
         <f t="shared" ref="H6:AM6" ca="1" si="3">LEFT(TEXT(H5,"jjj"),1)</f>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="I6" s="39" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="J6" s="41" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="K6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="L6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="M6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="N6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="O6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="P6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="Q6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="R6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="S6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="T6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="U6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="V6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="W6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="X6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="Y6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="Z6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AA6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AB6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="AC6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="AD6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AE6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AF6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="AG6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AH6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AI6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="AJ6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="AK6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AL6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AM6" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="AN6" s="40" t="str">
         <f t="shared" ref="AN6:BK6" ca="1" si="4">LEFT(TEXT(AN5,"jjj"),1)</f>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AO6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AP6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="AQ6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="AR6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AS6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="AT6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="AU6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="AV6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="AW6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="AX6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="AY6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="AZ6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="BA6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="BB6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="BC6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="BD6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>j</v>
       </c>
       <c r="BE6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>l</v>
+        <v>v</v>
       </c>
       <c r="BF6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>s</v>
       </c>
       <c r="BG6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>m</v>
+        <v>d</v>
       </c>
       <c r="BH6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>j</v>
+        <v>l</v>
       </c>
       <c r="BI6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>v</v>
+        <v>m</v>
       </c>
       <c r="BJ6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>s</v>
+        <v>m</v>
       </c>
       <c r="BK6" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>d</v>
+        <v>j</v>
       </c>
     </row>
     <row r="7" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3549,9 +3549,9 @@
         <v>1</v>
       </c>
       <c r="G10" s="19"/>
-      <c r="H10" s="27">
+      <c r="H10" s="27" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E10,$F10=1),Marqueur_Jalon,"")),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I10" s="27" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E10,$F10=1),Marqueur_Jalon,"")),"")</f>
@@ -3792,9 +3792,9 @@
         <v>1</v>
       </c>
       <c r="G11" s="19"/>
-      <c r="H11" s="27">
+      <c r="H11" s="27" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E11,$F11=1),Marqueur_Jalon,"")),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="I11" s="49" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E11,$F11=1),Marqueur_Jalon,"")),"")</f>
@@ -5298,9 +5298,9 @@
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="V17" s="27">
+      <c r="V17" s="27" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="W17" s="27" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
@@ -5476,13 +5476,13 @@
         <v>54</v>
       </c>
       <c r="D18" s="23">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E18" s="24">
-        <v>44095</v>
+        <v>44117</v>
       </c>
       <c r="F18" s="44">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="27" t="str">
@@ -6028,7 +6028,7 @@
         <v>44131</v>
       </c>
       <c r="F23" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="27"/>
@@ -6458,7 +6458,7 @@
         <v>59</v>
       </c>
       <c r="D29" s="23">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E29" s="24">
         <v>44095</v>
@@ -6533,7 +6533,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="23">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E30" s="24">
         <v>44131</v>
@@ -6592,9 +6592,9 @@
       <c r="BC30" s="27"/>
       <c r="BD30" s="27"/>
       <c r="BE30" s="27"/>
-      <c r="BF30" s="27">
+      <c r="BF30" s="27" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E30,$F30=1),Marqueur_Jalon,"")),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="BG30" s="27"/>
       <c r="BH30" s="27"/>
@@ -7890,7 +7890,7 @@
       <formula>AND(BF$5&gt;=$E30+1,BF$5&lt;=$E30+$F30-2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Incrément de défilement" prompt="La modification de ce nombre entraînera la défilement du diagramme de Gantt." sqref="E3">
       <formula1>0</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
GANTT A JOUR 27/10
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -230,16 +230,10 @@
     <t>Connexion sécurisée</t>
   </si>
   <si>
-    <t>AMINE &amp; QUENTIN</t>
-  </si>
-  <si>
     <t xml:space="preserve"> AMINE</t>
   </si>
   <si>
     <t>BONUS : Envoi de mail automatique après inscription</t>
-  </si>
-  <si>
-    <t>Création page "Annonces"</t>
   </si>
   <si>
     <t>Rédaction de la documentation Développeur</t>
@@ -249,6 +243,9 @@
   </si>
   <si>
     <t>Création de la page "Contact"</t>
+  </si>
+  <si>
+    <t>Création page "Offres d'emploi"</t>
   </si>
 </sst>
 </file>
@@ -2339,8 +2336,8 @@
   </sheetPr>
   <dimension ref="A1:BK46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5875,7 +5872,7 @@
         <v>44095</v>
       </c>
       <c r="F21" s="44">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="27"/>
@@ -6016,7 +6013,7 @@
     <row r="23" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12"/>
       <c r="B23" s="51" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>56</v>
@@ -6091,19 +6088,19 @@
     <row r="24" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="64" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>55</v>
       </c>
       <c r="D24" s="23">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E24" s="24">
         <v>44116</v>
       </c>
       <c r="F24" s="44">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G24" s="19"/>
       <c r="H24" s="27"/>
@@ -6166,17 +6163,19 @@
     <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="64" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D25" s="23">
-        <v>0</v>
-      </c>
-      <c r="E25" s="24"/>
+        <v>0.8</v>
+      </c>
+      <c r="E25" s="24">
+        <v>44131</v>
+      </c>
       <c r="F25" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="27"/>
@@ -6239,17 +6238,19 @@
     <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
       <c r="B26" s="64" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>55</v>
       </c>
       <c r="D26" s="23">
-        <v>0</v>
-      </c>
-      <c r="E26" s="24"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="24">
+        <v>44131</v>
+      </c>
       <c r="F26" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="27"/>
@@ -6455,7 +6456,7 @@
         <v>40</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" s="23">
         <v>0.8</v>
@@ -6530,7 +6531,7 @@
         <v>41</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" s="23">
         <v>0.6</v>
@@ -7723,7 +7724,7 @@
     </row>
     <row r="44" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="66" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="26" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
remise à niveau de l'insertion de l'heure lors de la connexion
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07F100F-0CED-4D81-9454-373BF0738DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="415"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <definedName name="Incrément_Défilement">Gantt!$E$3</definedName>
     <definedName name="Marqueur_Jalon">Gantt!$E$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -254,7 +255,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
@@ -1304,7 +1305,7 @@
     <cellStyle name="Avertissement" xfId="23" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="20" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="21" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="9"/>
+    <cellStyle name="Date" xfId="9" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Entrée" xfId="18" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="16" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -1326,7 +1327,7 @@
     <cellStyle name="Titre 4" xfId="11" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="25" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="22" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="zHiddenText" xfId="3"/>
+    <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
   <dxfs count="36">
     <dxf>
@@ -1933,12 +1934,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Gantt Table Style" pivot="0" count="3">
+    <tableStyle name="Gantt Table Style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="35"/>
       <tableStyleElement type="headerRow" dxfId="34"/>
       <tableStyleElement type="firstRowStripe" dxfId="33"/>
     </tableStyle>
-    <tableStyle name="ToDoList" pivot="0" count="9">
+    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="32"/>
       <tableStyleElement type="headerRow" dxfId="31"/>
       <tableStyleElement type="totalRow" dxfId="30"/>
@@ -2042,11 +2043,11 @@
           <xdr:col>7</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>31750</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>184150</xdr:colOff>
+          <xdr:colOff>180975</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>342900</xdr:rowOff>
         </xdr:to>
@@ -2089,8 +2090,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Jalons" displayName="Jalons" ref="B6:F43" totalsRowShown="0">
-  <autoFilter ref="B6:F43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Jalons" displayName="Jalons" ref="B6:F43" totalsRowShown="0">
+  <autoFilter ref="B6:F43" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2098,11 +2099,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Description du jalon"/>
-    <tableColumn id="3" name="Affecté à"/>
-    <tableColumn id="4" name="Avancement"/>
-    <tableColumn id="5" name="Début"/>
-    <tableColumn id="6" name="Nombre de jours"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Description du jalon"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Affecté à"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Avancement"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Début"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nombre de jours"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -2375,30 +2376,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BK45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" customWidth="1"/>
-    <col min="3" max="3" width="20.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="2.7265625" customWidth="1"/>
-    <col min="8" max="63" width="3.54296875" customWidth="1"/>
-    <col min="68" max="69" width="10.26953125"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="63" width="3.5703125" customWidth="1"/>
+    <col min="68" max="69" width="10.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="50.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:63" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2411,7 +2412,7 @@
       <c r="I1" s="18"/>
       <c r="AF1" s="18"/>
     </row>
-    <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -2434,7 +2435,7 @@
       <c r="M2" s="32"/>
       <c r="N2" s="32"/>
     </row>
-    <row r="3" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
@@ -2455,7 +2456,7 @@
       <c r="L3" s="43"/>
       <c r="M3" s="42"/>
     </row>
-    <row r="4" spans="1:63" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:63" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
@@ -2551,7 +2552,7 @@
       <c r="BJ4" s="17"/>
       <c r="BK4" s="17"/>
     </row>
-    <row r="5" spans="1:63" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
@@ -2782,7 +2783,7 @@
         <v>44166</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:63" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="7" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
@@ -3093,7 +3094,7 @@
       <c r="BJ7" s="37"/>
       <c r="BK7" s="37"/>
     </row>
-    <row r="8" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -3330,7 +3331,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="62" t="s">
         <v>21</v>
@@ -3573,7 +3574,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="28" t="s">
         <v>22</v>
@@ -3816,7 +3817,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="62" t="s">
         <v>23</v>
@@ -4059,7 +4060,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="28" t="s">
         <v>38</v>
@@ -4302,7 +4303,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="62" t="s">
         <v>24</v>
@@ -4545,7 +4546,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="53" t="s">
         <v>37</v>
@@ -4780,7 +4781,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="62" t="s">
         <v>26</v>
@@ -5023,7 +5024,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="50" t="s">
         <v>27</v>
@@ -5266,7 +5267,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="50" t="s">
         <v>28</v>
@@ -5509,7 +5510,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="50" t="s">
         <v>29</v>
@@ -5752,7 +5753,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="50" t="s">
         <v>30</v>
@@ -5827,7 +5828,7 @@
       <c r="BJ19" s="27"/>
       <c r="BK19" s="27"/>
     </row>
-    <row r="20" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="63" t="s">
         <v>32</v>
@@ -5902,7 +5903,7 @@
       <c r="BJ20" s="27"/>
       <c r="BK20" s="27"/>
     </row>
-    <row r="21" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="51" t="s">
         <v>33</v>
@@ -5980,7 +5981,7 @@
       <c r="BJ21" s="27"/>
       <c r="BK21" s="27"/>
     </row>
-    <row r="22" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="51" t="s">
         <v>57</v>
@@ -6055,7 +6056,7 @@
       <c r="BJ22" s="27"/>
       <c r="BK22" s="27"/>
     </row>
-    <row r="23" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="51" t="s">
         <v>60</v>
@@ -6130,7 +6131,7 @@
       <c r="BJ23" s="27"/>
       <c r="BK23" s="27"/>
     </row>
-    <row r="24" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="64" t="s">
         <v>61</v>
@@ -6205,7 +6206,7 @@
       <c r="BJ24" s="27"/>
       <c r="BK24" s="27"/>
     </row>
-    <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="64" t="s">
         <v>63</v>
@@ -6280,7 +6281,7 @@
       <c r="BJ25" s="27"/>
       <c r="BK25" s="27"/>
     </row>
-    <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="64" t="s">
         <v>62</v>
@@ -6355,7 +6356,7 @@
       <c r="BJ26" s="27"/>
       <c r="BK26" s="27"/>
     </row>
-    <row r="27" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="64" t="s">
         <v>31</v>
@@ -6430,7 +6431,7 @@
       <c r="BJ27" s="27"/>
       <c r="BK27" s="27"/>
     </row>
-    <row r="28" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="56" t="s">
         <v>39</v>
@@ -6497,7 +6498,7 @@
       <c r="BJ28" s="27"/>
       <c r="BK28" s="27"/>
     </row>
-    <row r="29" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="54" t="s">
         <v>40</v>
@@ -6572,7 +6573,7 @@
       <c r="BJ29" s="27"/>
       <c r="BK29" s="27"/>
     </row>
-    <row r="30" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="65" t="s">
         <v>41</v>
@@ -6650,7 +6651,7 @@
       <c r="BJ30" s="27"/>
       <c r="BK30" s="27"/>
     </row>
-    <row r="31" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="51" t="s">
         <v>42</v>
@@ -6721,7 +6722,7 @@
       <c r="BJ31" s="27"/>
       <c r="BK31" s="27"/>
     </row>
-    <row r="32" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="B32" s="57" t="s">
         <v>43</v>
@@ -6788,7 +6789,7 @@
       <c r="BJ32" s="27"/>
       <c r="BK32" s="27"/>
     </row>
-    <row r="33" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="50" t="s">
         <v>44</v>
@@ -6797,7 +6798,7 @@
         <v>56</v>
       </c>
       <c r="D33" s="23">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="E33" s="24">
         <v>44151</v>
@@ -6863,7 +6864,7 @@
       <c r="BJ33" s="27"/>
       <c r="BK33" s="27"/>
     </row>
-    <row r="34" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="50" t="s">
         <v>45</v>
@@ -6938,7 +6939,7 @@
       <c r="BJ34" s="27"/>
       <c r="BK34" s="27"/>
     </row>
-    <row r="35" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="51" t="s">
         <v>47</v>
@@ -7009,7 +7010,7 @@
       <c r="BJ35" s="27"/>
       <c r="BK35" s="27"/>
     </row>
-    <row r="36" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="64" t="s">
         <v>49</v>
@@ -7080,7 +7081,7 @@
       <c r="BJ36" s="27"/>
       <c r="BK36" s="27"/>
     </row>
-    <row r="37" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="51" t="s">
         <v>48</v>
@@ -7151,7 +7152,7 @@
       <c r="BJ37" s="27"/>
       <c r="BK37" s="27"/>
     </row>
-    <row r="38" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="B38" s="51" t="s">
         <v>46</v>
@@ -7226,7 +7227,7 @@
       <c r="BJ38" s="27"/>
       <c r="BK38" s="27"/>
     </row>
-    <row r="39" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="58" t="s">
         <v>50</v>
@@ -7463,7 +7464,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="60" t="s">
         <v>51</v>
@@ -7700,7 +7701,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="59" t="s">
         <v>52</v>
       </c>
@@ -7712,7 +7713,7 @@
       <c r="F41" s="44"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>8</v>
       </c>
@@ -7726,7 +7727,7 @@
       <c r="E42" s="24"/>
       <c r="F42" s="44"/>
     </row>
-    <row r="43" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="66" t="s">
         <v>59</v>
       </c>
@@ -7743,11 +7744,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="5"/>
       <c r="F44" s="14"/>
     </row>
-    <row r="45" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="6"/>
     </row>
   </sheetData>
@@ -7906,7 +7907,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Incrément de défilement" prompt="La modification de ce nombre entraînera la défilement du diagramme de Gantt." sqref="E3">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Incrément de défilement" prompt="La modification de ce nombre entraînera la défilement du diagramme de Gantt." sqref="E3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -7930,11 +7931,11 @@
                     <xdr:col>7</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>31750</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>12</xdr:col>
-                    <xdr:colOff>184150</xdr:colOff>
+                    <xdr:colOff>180975</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>342900</xdr:rowOff>
                   </to>
@@ -8046,35 +8047,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.1796875" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9.1796875" style="8"/>
+    <col min="1" max="1" width="87.140625" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" s="10" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>20</v>
       </c>

</xml_diff>